<commit_message>
line profile 사진 추가
</commit_message>
<xml_diff>
--- a/dsfgd.xlsx
+++ b/dsfgd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="현재_통합_문서" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seonjae Lee\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Thesis_Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -696,11 +696,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-46368864"/>
-        <c:axId val="-46380832"/>
+        <c:axId val="959419248"/>
+        <c:axId val="959419792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-46368864"/>
+        <c:axId val="959419248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +743,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-46380832"/>
+        <c:crossAx val="959419792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -751,7 +751,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-46380832"/>
+        <c:axId val="959419792"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -803,7 +803,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-46368864"/>
+        <c:crossAx val="959419248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -879,7 +879,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1573,8 +1573,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-45410352"/>
-        <c:axId val="-45404368"/>
+        <c:axId val="750426256"/>
+        <c:axId val="750426800"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1709,7 +1709,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$14:$D$21</c15:sqref>
@@ -1748,7 +1748,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$14:$E$21</c15:sqref>
@@ -1823,7 +1823,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$25:$D$60</c15:sqref>
@@ -1946,7 +1946,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$25:$E$60</c15:sqref>
@@ -2105,7 +2105,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$D$65:$D$90</c15:sqref>
@@ -2198,7 +2198,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Sheet1!$E$65:$E$90</c15:sqref>
@@ -2296,7 +2296,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-45410352"/>
+        <c:axId val="750426256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2354,12 +2354,12 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-45404368"/>
+        <c:crossAx val="750426800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-45404368"/>
+        <c:axId val="750426800"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2418,7 +2418,7 @@
             <a:endParaRPr lang="ko-KR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-45410352"/>
+        <c:crossAx val="750426256"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2480,12 +2480,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -2503,7 +2498,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
   <c:userShapes r:id="rId3"/>
 </c:chartSpace>
@@ -3612,16 +3607,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3642,16 +3637,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3684,8 +3679,8 @@
       <cdr:x>0.60205</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1"/>
@@ -3755,7 +3750,7 @@
           </cdr:txBody>
         </cdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <cdr:sp macro="" textlink="">
           <cdr:nvSpPr>
             <cdr:cNvPr id="2" name="TextBox 1"/>
@@ -3806,12 +3801,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0262</cdr:x>
-      <cdr:y>0.11456</cdr:y>
+      <cdr:x>0.0219</cdr:x>
+      <cdr:y>0.0358</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.07796</cdr:x>
-      <cdr:y>0.80668</cdr:y>
+      <cdr:x>0.07366</cdr:x>
+      <cdr:y>0.78997</cdr:y>
     </cdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -3822,8 +3817,8 @@
           </cdr:nvSpPr>
           <cdr:spPr>
             <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-              <a:off x="-828285" y="1333195"/>
-              <a:ext cx="2209800" cy="274930"/>
+              <a:off x="-950212" y="1180804"/>
+              <a:ext cx="2407913" cy="274904"/>
             </a:xfrm>
             <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
               <a:avLst/>
@@ -3872,11 +3867,14 @@
                     </m:sub>
                   </m:sSub>
                   <m:r>
-                    <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0" i="1">
+                    <m:rPr>
+                      <m:nor/>
+                    </m:rPr>
+                    <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0" i="0">
                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     </a:rPr>
-                    <m:t>𝑘𝑚</m:t>
+                    <m:t>km</m:t>
                   </m:r>
                   <m:sSup>
                     <m:sSupPr>
@@ -3893,7 +3891,17 @@
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑠</m:t>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>s</m:t>
                       </m:r>
                     </m:e>
                     <m:sup>
@@ -3921,7 +3929,17 @@
                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                         </a:rPr>
-                        <m:t>𝑦𝑟</m:t>
+                        <m:t> </m:t>
+                      </m:r>
+                      <m:r>
+                        <m:rPr>
+                          <m:nor/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>yr</m:t>
                       </m:r>
                     </m:e>
                     <m:sup>
@@ -3955,8 +3973,8 @@
           </cdr:nvSpPr>
           <cdr:spPr>
             <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
-              <a:off x="-828285" y="1333195"/>
-              <a:ext cx="2209800" cy="274930"/>
+              <a:off x="-950212" y="1180804"/>
+              <a:ext cx="2407913" cy="274904"/>
             </a:xfrm>
             <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
               <a:avLst/>
@@ -3988,7 +4006,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t> 𝑘𝑚𝑠^(−1) 〖𝑦𝑟〗^(−1)</a:t>
+                <a:t> "km" 〖 "s" 〗^(−1) 〖 "yr" 〗^(−1)</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="en-US" altLang="ko-KR" sz="1100" b="0" i="0">
@@ -4272,8 +4290,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4334,7 +4352,7 @@
         <v>48.11</v>
       </c>
       <c r="N2" s="1">
-        <f>B2+C2</f>
+        <f t="shared" ref="N2:N12" si="0">B2+C2</f>
         <v>1.3208E-3</v>
       </c>
       <c r="O2" t="s">
@@ -4367,7 +4385,7 @@
         <v>2.1299999999999999E-5</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F33" si="0">LOG(D3)</f>
+        <f t="shared" ref="F3:F33" si="1">LOG(D3)</f>
         <v>1.1989318699322091</v>
       </c>
       <c r="G3" s="2">
@@ -4383,11 +4401,11 @@
         <v>2.1299999999999999E-5</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M66" si="1">D3</f>
+        <f t="shared" ref="M3:M66" si="2">D3</f>
         <v>15.81</v>
       </c>
       <c r="N3" s="1">
-        <f>B3+C3</f>
+        <f t="shared" si="0"/>
         <v>2.2060000000000001E-3</v>
       </c>
       <c r="O3" t="s">
@@ -4420,7 +4438,7 @@
         <v>5.6400000000000002E-5</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.303412070596742</v>
       </c>
       <c r="G4" s="2">
@@ -4436,11 +4454,11 @@
         <v>5.6400000000000002E-5</v>
       </c>
       <c r="M4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.11</v>
       </c>
       <c r="N4" s="1">
-        <f>B4+C4</f>
+        <f t="shared" si="0"/>
         <v>2.5899999999999999E-3</v>
       </c>
       <c r="O4" t="s">
@@ -4470,7 +4488,7 @@
         <v>4.4199999999999997E-5</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75434833571101889</v>
       </c>
       <c r="G5" s="2">
@@ -4486,11 +4504,11 @@
         <v>4.4199999999999997E-5</v>
       </c>
       <c r="M5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.68</v>
       </c>
       <c r="N5" s="1">
-        <f>B5+C5</f>
+        <f t="shared" si="0"/>
         <v>2.9908999999999999E-3</v>
       </c>
       <c r="O5" t="s">
@@ -4523,7 +4541,7 @@
         <v>1.2199999999999999E-3</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5573387447859153</v>
       </c>
       <c r="G6" s="2">
@@ -4539,11 +4557,11 @@
         <v>1.12E-4</v>
       </c>
       <c r="M6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>360.86</v>
       </c>
       <c r="N6" s="1">
-        <f>B6+C6</f>
+        <f t="shared" si="0"/>
         <v>8.4770000000000002E-3</v>
       </c>
       <c r="O6" t="s">
@@ -4576,7 +4594,7 @@
         <v>2.3099999999999999E-5</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3410386316775229</v>
       </c>
       <c r="G7" s="2">
@@ -4592,11 +4610,11 @@
         <v>2.3099999999999999E-5</v>
       </c>
       <c r="M7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.93</v>
       </c>
       <c r="N7" s="1">
-        <f>B7+C7</f>
+        <f t="shared" si="0"/>
         <v>5.9619999999999996E-4</v>
       </c>
       <c r="O7" t="s">
@@ -4629,7 +4647,7 @@
         <v>1.4600000000000001E-5</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.94987770403687477</v>
       </c>
       <c r="G8" s="2">
@@ -4645,11 +4663,11 @@
         <v>1.4600000000000001E-5</v>
       </c>
       <c r="M8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.91</v>
       </c>
       <c r="N8" s="1">
-        <f>B8+C8</f>
+        <f t="shared" si="0"/>
         <v>1.8228999999999999E-3</v>
       </c>
     </row>
@@ -4658,11 +4676,11 @@
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="M9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N9" s="1">
-        <f>B9+C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4671,11 +4689,11 @@
       <c r="C10" s="1"/>
       <c r="E10" s="1"/>
       <c r="M10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N10" s="1">
-        <f>B10+C10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4684,11 +4702,11 @@
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="M11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <f>B11+C11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4697,11 +4715,11 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="M12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <f>B12+C12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -4728,11 +4746,11 @@
         <v>20.11</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ref="E3:E66" si="2">B14+C14</f>
+        <f t="shared" ref="E14:E66" si="3">B14+C14</f>
         <v>2.0240000000000001E-4</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.303412070596742</v>
       </c>
       <c r="G14" s="1">
@@ -4740,11 +4758,11 @@
         <v>2.0240000000000001E-4</v>
       </c>
       <c r="M14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.11</v>
       </c>
       <c r="N14" s="1">
-        <f>B14+C14</f>
+        <f t="shared" ref="N14:N21" si="4">B14+C14</f>
         <v>2.0240000000000001E-4</v>
       </c>
     </row>
@@ -4762,23 +4780,23 @@
         <v>15.81</v>
       </c>
       <c r="E15" s="1">
+        <f t="shared" si="3"/>
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1.1989318699322091</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" ref="G15:G21" si="5">B15+C15</f>
+        <v>8.7000000000000001E-5</v>
+      </c>
+      <c r="M15">
         <f t="shared" si="2"/>
-        <v>8.7000000000000001E-5</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1.1989318699322091</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" ref="G15:G21" si="3">B15+C15</f>
-        <v>8.7000000000000001E-5</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="1"/>
         <v>15.81</v>
       </c>
       <c r="N15" s="1">
-        <f>B15+C15</f>
+        <f t="shared" si="4"/>
         <v>8.7000000000000001E-5</v>
       </c>
     </row>
@@ -4796,23 +4814,23 @@
         <v>48.11</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="2"/>
-        <v>3.8699999999999999E-5</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>1.6822353569025641</v>
-      </c>
-      <c r="G16" s="1">
         <f t="shared" si="3"/>
         <v>3.8699999999999999E-5</v>
       </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>1.6822353569025641</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="5"/>
+        <v>3.8699999999999999E-5</v>
+      </c>
       <c r="M16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>48.11</v>
       </c>
       <c r="N16" s="1">
-        <f>B16+C16</f>
+        <f t="shared" si="4"/>
         <v>3.8699999999999999E-5</v>
       </c>
     </row>
@@ -4830,23 +4848,23 @@
         <v>8.91</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="2"/>
-        <v>4.4000000000000002E-4</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0.94987770403687477</v>
-      </c>
-      <c r="G17" s="1">
         <f t="shared" si="3"/>
         <v>4.4000000000000002E-4</v>
       </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0.94987770403687477</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="5"/>
+        <v>4.4000000000000002E-4</v>
+      </c>
       <c r="M17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.91</v>
       </c>
       <c r="N17" s="1">
-        <f>B17+C17</f>
+        <f t="shared" si="4"/>
         <v>4.4000000000000002E-4</v>
       </c>
     </row>
@@ -4864,23 +4882,23 @@
         <v>5.68</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="2"/>
-        <v>1.44E-4</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>0.75434833571101889</v>
-      </c>
-      <c r="G18" s="1">
         <f t="shared" si="3"/>
         <v>1.44E-4</v>
       </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>0.75434833571101889</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="5"/>
+        <v>1.44E-4</v>
+      </c>
       <c r="M18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.68</v>
       </c>
       <c r="N18" s="1">
-        <f>B18+C18</f>
+        <f t="shared" si="4"/>
         <v>1.44E-4</v>
       </c>
     </row>
@@ -4898,23 +4916,23 @@
         <v>360.86</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="2"/>
-        <v>2.3730000000000001E-3</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>2.5573387447859153</v>
-      </c>
-      <c r="G19" s="1">
         <f t="shared" si="3"/>
         <v>2.3730000000000001E-3</v>
       </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>2.5573387447859153</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="5"/>
+        <v>2.3730000000000001E-3</v>
+      </c>
       <c r="M19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>360.86</v>
       </c>
       <c r="N19" s="1">
-        <f>B19+C19</f>
+        <f t="shared" si="4"/>
         <v>2.3730000000000001E-3</v>
       </c>
     </row>
@@ -4932,23 +4950,23 @@
         <v>100</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" si="2"/>
-        <v>8.4000000000000009E-5</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G20" s="1">
         <f t="shared" si="3"/>
         <v>8.4000000000000009E-5</v>
       </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="5"/>
+        <v>8.4000000000000009E-5</v>
+      </c>
       <c r="M20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100</v>
       </c>
       <c r="N20" s="1">
-        <f>B20+C20</f>
+        <f t="shared" si="4"/>
         <v>8.4000000000000009E-5</v>
       </c>
     </row>
@@ -4966,23 +4984,23 @@
         <v>21.93</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="2"/>
-        <v>9.7999999999999997E-5</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>1.3410386316775229</v>
-      </c>
-      <c r="G21" s="1">
         <f t="shared" si="3"/>
         <v>9.7999999999999997E-5</v>
       </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1.3410386316775229</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="5"/>
+        <v>9.7999999999999997E-5</v>
+      </c>
       <c r="M21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>21.93</v>
       </c>
       <c r="N21" s="1">
-        <f>B21+C21</f>
+        <f t="shared" si="4"/>
         <v>9.7999999999999997E-5</v>
       </c>
     </row>
@@ -5017,19 +5035,19 @@
         <v>3.7</v>
       </c>
       <c r="E25" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3499999999999999E-5</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.56820172406699498</v>
+      </c>
+      <c r="M25">
         <f t="shared" si="2"/>
-        <v>1.3499999999999999E-5</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>0.56820172406699498</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="1"/>
         <v>3.7</v>
       </c>
       <c r="N25" s="1">
-        <f>B25+C25</f>
+        <f t="shared" ref="N25:N33" si="6">B25+C25</f>
         <v>1.3499999999999999E-5</v>
       </c>
     </row>
@@ -5047,19 +5065,19 @@
         <v>25.5</v>
       </c>
       <c r="E26" s="1">
+        <f t="shared" si="3"/>
+        <v>7.3000000000000013E-5</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>1.4065401804339552</v>
+      </c>
+      <c r="M26">
         <f t="shared" si="2"/>
-        <v>7.3000000000000013E-5</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>1.4065401804339552</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="1"/>
         <v>25.5</v>
       </c>
       <c r="N26" s="1">
-        <f>B26+C26</f>
+        <f t="shared" si="6"/>
         <v>7.3000000000000013E-5</v>
       </c>
     </row>
@@ -5077,19 +5095,19 @@
         <v>6.98</v>
       </c>
       <c r="E27" s="1">
+        <f t="shared" si="3"/>
+        <v>9.3999999999999998E-6</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0.84385542262316116</v>
+      </c>
+      <c r="M27">
         <f t="shared" si="2"/>
-        <v>9.3999999999999998E-6</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>0.84385542262316116</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="1"/>
         <v>6.98</v>
       </c>
       <c r="N27" s="1">
-        <f>B27+C27</f>
+        <f t="shared" si="6"/>
         <v>9.3999999999999998E-6</v>
       </c>
     </row>
@@ -5107,19 +5125,19 @@
         <v>21.9</v>
       </c>
       <c r="E28" s="1">
+        <f t="shared" si="3"/>
+        <v>2.1900000000000001E-3</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1.3404441148401183</v>
+      </c>
+      <c r="M28">
         <f t="shared" si="2"/>
-        <v>2.1900000000000001E-3</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>1.3404441148401183</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="1"/>
         <v>21.9</v>
       </c>
       <c r="N28" s="1">
-        <f>B28+C28</f>
+        <f t="shared" si="6"/>
         <v>2.1900000000000001E-3</v>
       </c>
     </row>
@@ -5137,19 +5155,19 @@
         <v>0.7</v>
       </c>
       <c r="E29" s="1">
+        <f t="shared" si="3"/>
+        <v>1.8999999999999998E-7</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>-0.15490195998574319</v>
+      </c>
+      <c r="M29">
         <f t="shared" si="2"/>
-        <v>1.8999999999999998E-7</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>-0.15490195998574319</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="N29" s="1">
-        <f>B29+C29</f>
+        <f t="shared" si="6"/>
         <v>1.8999999999999998E-7</v>
       </c>
     </row>
@@ -5167,19 +5185,19 @@
         <v>2.9</v>
       </c>
       <c r="E30" s="1">
+        <f t="shared" si="3"/>
+        <v>3.7000000000000002E-6</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>0.46239799789895608</v>
+      </c>
+      <c r="M30">
         <f t="shared" si="2"/>
-        <v>3.7000000000000002E-6</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>0.46239799789895608</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
       <c r="N30" s="1">
-        <f>B30+C30</f>
+        <f t="shared" si="6"/>
         <v>3.7000000000000002E-6</v>
       </c>
     </row>
@@ -5197,19 +5215,19 @@
         <v>0.66</v>
       </c>
       <c r="E31" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6400000000000001E-6</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>-0.18045606445813131</v>
+      </c>
+      <c r="M31">
         <f t="shared" si="2"/>
-        <v>2.6400000000000001E-6</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>-0.18045606445813131</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="1"/>
         <v>0.66</v>
       </c>
       <c r="N31" s="1">
-        <f>B31+C31</f>
+        <f t="shared" si="6"/>
         <v>2.6400000000000001E-6</v>
       </c>
     </row>
@@ -5227,19 +5245,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E32" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2799999999999999E-4</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>0.34242268082220628</v>
+      </c>
+      <c r="M32">
         <f t="shared" si="2"/>
-        <v>1.2799999999999999E-4</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>0.34242268082220628</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="1"/>
         <v>2.2000000000000002</v>
       </c>
       <c r="N32" s="1">
-        <f>B32+C32</f>
+        <f t="shared" si="6"/>
         <v>1.2799999999999999E-4</v>
       </c>
     </row>
@@ -5257,19 +5275,19 @@
         <v>1.3</v>
       </c>
       <c r="E33" s="1">
+        <f t="shared" si="3"/>
+        <v>4.3300000000000002E-5</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>0.11394335230683679</v>
+      </c>
+      <c r="M33">
         <f t="shared" si="2"/>
-        <v>4.3300000000000002E-5</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>0.11394335230683679</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="N33" s="1">
-        <f>B33+C33</f>
+        <f t="shared" si="6"/>
         <v>4.3300000000000002E-5</v>
       </c>
     </row>
@@ -5282,11 +5300,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ref="E34" si="4">B34+C34</f>
+        <f t="shared" ref="E34" si="7">B34+C34</f>
         <v>1.1E-5</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34" si="5">LOG10(D34)</f>
+        <f t="shared" ref="F34" si="8">LOG10(D34)</f>
         <v>0.36172783601759284</v>
       </c>
       <c r="N34" s="1"/>
@@ -5302,7 +5320,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1E-4</v>
       </c>
       <c r="F35">
@@ -5310,11 +5328,11 @@
         <v>1</v>
       </c>
       <c r="M35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="N35" s="1">
-        <f>B35+C35</f>
+        <f t="shared" ref="N35:N60" si="9">B35+C35</f>
         <v>1E-4</v>
       </c>
     </row>
@@ -5329,19 +5347,19 @@
         <v>9</v>
       </c>
       <c r="E36" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:F90" si="10">LOG10(D36)</f>
+        <v>0.95424250943932487</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="2"/>
-        <v>1.3999999999999999E-4</v>
-      </c>
-      <c r="F36">
-        <f t="shared" ref="F36:F90" si="6">LOG10(D36)</f>
-        <v>0.95424250943932487</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="N36" s="1">
-        <f>B36+C36</f>
+        <f t="shared" si="9"/>
         <v>1.3999999999999999E-4</v>
       </c>
     </row>
@@ -5356,19 +5374,19 @@
         <v>1.5</v>
       </c>
       <c r="E37" s="1">
+        <f t="shared" si="3"/>
+        <v>6.7999999999999999E-5</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="10"/>
+        <v>0.17609125905568124</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="2"/>
-        <v>6.7999999999999999E-5</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="6"/>
-        <v>0.17609125905568124</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="N37" s="1">
-        <f>B37+C37</f>
+        <f t="shared" si="9"/>
         <v>6.7999999999999999E-5</v>
       </c>
     </row>
@@ -5383,19 +5401,19 @@
         <v>9.4</v>
       </c>
       <c r="E38" s="1">
+        <f t="shared" si="3"/>
+        <v>4.1E-5</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="10"/>
+        <v>0.97312785359969867</v>
+      </c>
+      <c r="M38">
         <f t="shared" si="2"/>
-        <v>4.1E-5</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="6"/>
-        <v>0.97312785359969867</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="1"/>
         <v>9.4</v>
       </c>
       <c r="N38" s="1">
-        <f>B38+C38</f>
+        <f t="shared" si="9"/>
         <v>4.1E-5</v>
       </c>
     </row>
@@ -5410,19 +5428,19 @@
         <v>0.4</v>
       </c>
       <c r="E39" s="1">
+        <f t="shared" si="3"/>
+        <v>3.1E-6</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="10"/>
+        <v>-0.3979400086720376</v>
+      </c>
+      <c r="M39">
         <f t="shared" si="2"/>
-        <v>3.1E-6</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="6"/>
-        <v>-0.3979400086720376</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="N39" s="1">
-        <f>B39+C39</f>
+        <f t="shared" si="9"/>
         <v>3.1E-6</v>
       </c>
     </row>
@@ -5437,19 +5455,19 @@
         <v>1.4</v>
       </c>
       <c r="E40" s="1">
+        <f t="shared" si="3"/>
+        <v>5.6999999999999996E-6</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="10"/>
+        <v>0.14612803567823801</v>
+      </c>
+      <c r="M40">
         <f t="shared" si="2"/>
-        <v>5.6999999999999996E-6</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="6"/>
-        <v>0.14612803567823801</v>
-      </c>
-      <c r="M40">
-        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
       <c r="N40" s="1">
-        <f>B40+C40</f>
+        <f t="shared" si="9"/>
         <v>5.6999999999999996E-6</v>
       </c>
     </row>
@@ -5464,19 +5482,19 @@
         <v>0.5</v>
       </c>
       <c r="E41" s="1">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000001E-6</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="10"/>
+        <v>-0.3010299956639812</v>
+      </c>
+      <c r="M41">
         <f t="shared" si="2"/>
-        <v>2.2000000000000001E-6</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="6"/>
-        <v>-0.3010299956639812</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="N41" s="1">
-        <f>B41+C41</f>
+        <f t="shared" si="9"/>
         <v>2.2000000000000001E-6</v>
       </c>
     </row>
@@ -5491,19 +5509,19 @@
         <v>0.3</v>
       </c>
       <c r="E42" s="1">
+        <f t="shared" si="3"/>
+        <v>3.1E-6</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="10"/>
+        <v>-0.52287874528033762</v>
+      </c>
+      <c r="M42">
         <f t="shared" si="2"/>
-        <v>3.1E-6</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="6"/>
-        <v>-0.52287874528033762</v>
-      </c>
-      <c r="M42">
-        <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
       <c r="N42" s="1">
-        <f>B42+C42</f>
+        <f t="shared" si="9"/>
         <v>3.1E-6</v>
       </c>
     </row>
@@ -5518,19 +5536,19 @@
         <v>2.4</v>
       </c>
       <c r="E43" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="10"/>
+        <v>0.38021124171160603</v>
+      </c>
+      <c r="M43">
         <f t="shared" si="2"/>
-        <v>1.5999999999999999E-5</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="6"/>
-        <v>0.38021124171160603</v>
-      </c>
-      <c r="M43">
-        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="N43" s="1">
-        <f>B43+C43</f>
+        <f t="shared" si="9"/>
         <v>1.5999999999999999E-5</v>
       </c>
     </row>
@@ -5545,19 +5563,19 @@
         <v>1.6</v>
       </c>
       <c r="E44" s="1">
+        <f t="shared" si="3"/>
+        <v>7.9000000000000006E-6</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="10"/>
+        <v>0.20411998265592479</v>
+      </c>
+      <c r="M44">
         <f t="shared" si="2"/>
-        <v>7.9000000000000006E-6</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="6"/>
-        <v>0.20411998265592479</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
       <c r="N44" s="1">
-        <f>B44+C44</f>
+        <f t="shared" si="9"/>
         <v>7.9000000000000006E-6</v>
       </c>
     </row>
@@ -5572,19 +5590,19 @@
         <v>0.7</v>
       </c>
       <c r="E45" s="1">
+        <f t="shared" si="3"/>
+        <v>5.6999999999999996E-6</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="10"/>
+        <v>-0.15490195998574319</v>
+      </c>
+      <c r="M45">
         <f t="shared" si="2"/>
-        <v>5.6999999999999996E-6</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="6"/>
-        <v>-0.15490195998574319</v>
-      </c>
-      <c r="M45">
-        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="N45" s="1">
-        <f>B45+C45</f>
+        <f t="shared" si="9"/>
         <v>5.6999999999999996E-6</v>
       </c>
     </row>
@@ -5599,19 +5617,19 @@
         <v>1</v>
       </c>
       <c r="E46" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3999999999999999E-4</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M46">
         <f t="shared" si="2"/>
-        <v>1.3999999999999999E-4</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N46" s="1">
-        <f>B46+C46</f>
+        <f t="shared" si="9"/>
         <v>1.3999999999999999E-4</v>
       </c>
     </row>
@@ -5626,19 +5644,19 @@
         <v>41</v>
       </c>
       <c r="E47" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5E-5</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="10"/>
+        <v>1.6127838567197355</v>
+      </c>
+      <c r="M47">
         <f t="shared" si="2"/>
-        <v>1.5E-5</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="6"/>
-        <v>1.6127838567197355</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="N47" s="1">
-        <f>B47+C47</f>
+        <f t="shared" si="9"/>
         <v>1.5E-5</v>
       </c>
     </row>
@@ -5653,19 +5671,19 @@
         <v>13</v>
       </c>
       <c r="E48" s="1">
+        <f t="shared" si="3"/>
+        <v>2.6999999999999999E-5</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="10"/>
+        <v>1.1139433523068367</v>
+      </c>
+      <c r="M48">
         <f t="shared" si="2"/>
-        <v>2.6999999999999999E-5</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="6"/>
-        <v>1.1139433523068367</v>
-      </c>
-      <c r="M48">
-        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="N48" s="1">
-        <f>B48+C48</f>
+        <f t="shared" si="9"/>
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
@@ -5680,19 +5698,19 @@
         <v>11.1</v>
       </c>
       <c r="E49" s="1">
+        <f t="shared" si="3"/>
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="10"/>
+        <v>1.0453229787866574</v>
+      </c>
+      <c r="M49">
         <f t="shared" si="2"/>
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="6"/>
-        <v>1.0453229787866574</v>
-      </c>
-      <c r="M49">
-        <f t="shared" si="1"/>
         <v>11.1</v>
       </c>
       <c r="N49" s="1">
-        <f>B49+C49</f>
+        <f t="shared" si="9"/>
         <v>3.0000000000000001E-5</v>
       </c>
     </row>
@@ -5707,19 +5725,19 @@
         <v>1.3</v>
       </c>
       <c r="E50" s="1">
+        <f t="shared" si="3"/>
+        <v>5.4999999999999999E-6</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="10"/>
+        <v>0.11394335230683679</v>
+      </c>
+      <c r="M50">
         <f t="shared" si="2"/>
-        <v>5.4999999999999999E-6</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="6"/>
-        <v>0.11394335230683679</v>
-      </c>
-      <c r="M50">
-        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
       <c r="N50" s="1">
-        <f>B50+C50</f>
+        <f t="shared" si="9"/>
         <v>5.4999999999999999E-6</v>
       </c>
     </row>
@@ -5734,19 +5752,19 @@
         <v>23</v>
       </c>
       <c r="E51" s="1">
+        <f t="shared" si="3"/>
+        <v>4.2000000000000002E-4</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="10"/>
+        <v>1.3617278360175928</v>
+      </c>
+      <c r="M51">
         <f t="shared" si="2"/>
-        <v>4.2000000000000002E-4</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="6"/>
-        <v>1.3617278360175928</v>
-      </c>
-      <c r="M51">
-        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="N51" s="1">
-        <f>B51+C51</f>
+        <f t="shared" si="9"/>
         <v>4.2000000000000002E-4</v>
       </c>
     </row>
@@ -5761,19 +5779,19 @@
         <v>14</v>
       </c>
       <c r="E52" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5E-5</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="10"/>
+        <v>1.146128035678238</v>
+      </c>
+      <c r="M52">
         <f t="shared" si="2"/>
-        <v>1.5E-5</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="6"/>
-        <v>1.146128035678238</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="N52" s="1">
-        <f>B52+C52</f>
+        <f t="shared" si="9"/>
         <v>1.5E-5</v>
       </c>
     </row>
@@ -5788,19 +5806,19 @@
         <v>3</v>
       </c>
       <c r="E53" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="10"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="M53">
         <f t="shared" si="2"/>
-        <v>3.6999999999999999E-4</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="6"/>
-        <v>0.47712125471966244</v>
-      </c>
-      <c r="M53">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N53" s="1">
-        <f>B53+C53</f>
+        <f t="shared" si="9"/>
         <v>3.6999999999999999E-4</v>
       </c>
     </row>
@@ -5815,19 +5833,19 @@
         <v>3</v>
       </c>
       <c r="E54" s="1">
+        <f t="shared" si="3"/>
+        <v>1.2E-5</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="10"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="M54">
         <f t="shared" si="2"/>
-        <v>1.2E-5</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="6"/>
-        <v>0.47712125471966244</v>
-      </c>
-      <c r="M54">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N54" s="1">
-        <f>B54+C54</f>
+        <f t="shared" si="9"/>
         <v>1.2E-5</v>
       </c>
     </row>
@@ -5842,19 +5860,19 @@
         <v>3.3</v>
       </c>
       <c r="E55" s="1">
+        <f t="shared" si="3"/>
+        <v>4.6999999999999999E-6</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="10"/>
+        <v>0.51851393987788741</v>
+      </c>
+      <c r="M55">
         <f t="shared" si="2"/>
-        <v>4.6999999999999999E-6</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="6"/>
-        <v>0.51851393987788741</v>
-      </c>
-      <c r="M55">
-        <f t="shared" si="1"/>
         <v>3.3</v>
       </c>
       <c r="N55" s="1">
-        <f>B55+C55</f>
+        <f t="shared" si="9"/>
         <v>4.6999999999999999E-6</v>
       </c>
     </row>
@@ -5869,19 +5887,19 @@
         <v>3</v>
       </c>
       <c r="E56" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="10"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="M56">
         <f t="shared" si="2"/>
-        <v>2.5000000000000001E-5</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="6"/>
-        <v>0.47712125471966244</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N56" s="1">
-        <f>B56+C56</f>
+        <f t="shared" si="9"/>
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
@@ -5896,19 +5914,19 @@
         <v>0.8</v>
       </c>
       <c r="E57" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7999999999999999E-6</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="10"/>
+        <v>-9.6910013008056392E-2</v>
+      </c>
+      <c r="M57">
         <f t="shared" si="2"/>
-        <v>2.7999999999999999E-6</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="6"/>
-        <v>-9.6910013008056392E-2</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="N57" s="1">
-        <f>B57+C57</f>
+        <f t="shared" si="9"/>
         <v>2.7999999999999999E-6</v>
       </c>
     </row>
@@ -5923,19 +5941,19 @@
         <v>2.4</v>
       </c>
       <c r="E58" s="1">
+        <f t="shared" si="3"/>
+        <v>2.8E-5</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="10"/>
+        <v>0.38021124171160603</v>
+      </c>
+      <c r="M58">
         <f t="shared" si="2"/>
-        <v>2.8E-5</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="6"/>
-        <v>0.38021124171160603</v>
-      </c>
-      <c r="M58">
-        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
       <c r="N58" s="1">
-        <f>B58+C58</f>
+        <f t="shared" si="9"/>
         <v>2.8E-5</v>
       </c>
     </row>
@@ -5950,19 +5968,19 @@
         <v>4.7</v>
       </c>
       <c r="E59" s="1">
+        <f t="shared" si="3"/>
+        <v>1.5E-5</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="10"/>
+        <v>0.67209785793571752</v>
+      </c>
+      <c r="M59">
         <f t="shared" si="2"/>
-        <v>1.5E-5</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="6"/>
-        <v>0.67209785793571752</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="1"/>
         <v>4.7</v>
       </c>
       <c r="N59" s="1">
-        <f>B59+C59</f>
+        <f t="shared" si="9"/>
         <v>1.5E-5</v>
       </c>
     </row>
@@ -5977,19 +5995,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E60" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1E-5</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="10"/>
+        <v>0.36172783601759284</v>
+      </c>
+      <c r="M60">
         <f t="shared" si="2"/>
-        <v>1.1E-5</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="6"/>
-        <v>0.36172783601759284</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
       <c r="N60" s="1">
-        <f>B60+C60</f>
+        <f t="shared" si="9"/>
         <v>1.1E-5</v>
       </c>
     </row>
@@ -6020,19 +6038,19 @@
         <v>1380</v>
       </c>
       <c r="E65" s="1">
+        <f t="shared" si="3"/>
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="10"/>
+        <v>3.1398790864012365</v>
+      </c>
+      <c r="M65">
         <f t="shared" si="2"/>
-        <v>2.7999999999999998E-4</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="6"/>
-        <v>3.1398790864012365</v>
-      </c>
-      <c r="M65">
-        <f t="shared" si="1"/>
         <v>1380</v>
       </c>
       <c r="N65" s="1">
-        <f>B65+C65</f>
+        <f t="shared" ref="N65:N90" si="11">B65+C65</f>
         <v>2.7999999999999998E-4</v>
       </c>
     </row>
@@ -6044,19 +6062,19 @@
         <v>51500</v>
       </c>
       <c r="E66" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4E-3</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="10"/>
+        <v>4.7118072290411908</v>
+      </c>
+      <c r="M66">
         <f t="shared" si="2"/>
-        <v>1.4E-3</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="6"/>
-        <v>4.7118072290411908</v>
-      </c>
-      <c r="M66">
-        <f t="shared" si="1"/>
         <v>51500</v>
       </c>
       <c r="N66" s="1">
-        <f>B66+C66</f>
+        <f t="shared" si="11"/>
         <v>1.4E-3</v>
       </c>
     </row>
@@ -6068,19 +6086,19 @@
         <v>56100</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E90" si="7">B67+C67</f>
+        <f t="shared" ref="E67:E90" si="12">B67+C67</f>
         <v>6.3E-3</v>
       </c>
       <c r="F67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.7489628612561612</v>
       </c>
       <c r="M67">
-        <f t="shared" ref="M67:M90" si="8">D67</f>
+        <f t="shared" ref="M67:M90" si="13">D67</f>
         <v>56100</v>
       </c>
       <c r="N67" s="1">
-        <f>B67+C67</f>
+        <f t="shared" si="11"/>
         <v>6.3E-3</v>
       </c>
     </row>
@@ -6092,19 +6110,19 @@
         <v>24000</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.5999999999999999E-3</v>
       </c>
       <c r="F68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.3802112417116064</v>
       </c>
       <c r="M68">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>24000</v>
       </c>
       <c r="N68" s="1">
-        <f>B68+C68</f>
+        <f t="shared" si="11"/>
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
@@ -6116,19 +6134,19 @@
         <v>1380</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="F69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.1398790864012365</v>
       </c>
       <c r="M69">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1380</v>
       </c>
       <c r="N69" s="1">
-        <f>B69+C69</f>
+        <f t="shared" si="11"/>
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
@@ -6140,19 +6158,19 @@
         <v>664</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.2999999999999999E-3</v>
       </c>
       <c r="F70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.8221680793680175</v>
       </c>
       <c r="M70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>664</v>
       </c>
       <c r="N70" s="1">
-        <f>B70+C70</f>
+        <f t="shared" si="11"/>
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
@@ -6164,19 +6182,19 @@
         <v>5830</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="F71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.7656685547590141</v>
       </c>
       <c r="M71">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>5830</v>
       </c>
       <c r="N71" s="1">
-        <f>B71+C71</f>
+        <f t="shared" si="11"/>
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
@@ -6188,19 +6206,19 @@
         <v>5830</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2E-3</v>
       </c>
       <c r="F72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.7656685547590141</v>
       </c>
       <c r="M72">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>5830</v>
       </c>
       <c r="N72" s="1">
-        <f>B72+C72</f>
+        <f t="shared" si="11"/>
         <v>2E-3</v>
       </c>
     </row>
@@ -6212,19 +6230,19 @@
         <v>9080</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.0999999999999999E-4</v>
       </c>
       <c r="F73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.958085848521085</v>
       </c>
       <c r="M73">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>9080</v>
       </c>
       <c r="N73" s="1">
-        <f>B73+C73</f>
+        <f t="shared" si="11"/>
         <v>4.0999999999999999E-4</v>
       </c>
     </row>
@@ -6236,19 +6254,19 @@
         <v>6640</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="F74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.8221680793680175</v>
       </c>
       <c r="M74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>6640</v>
       </c>
       <c r="N74" s="1">
-        <f>B74+C74</f>
+        <f t="shared" si="11"/>
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
@@ -6260,19 +6278,19 @@
         <v>20100</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.8999999999999998E-3</v>
       </c>
       <c r="F75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.3031960574204886</v>
       </c>
       <c r="M75">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>20100</v>
       </c>
       <c r="N75" s="1">
-        <f>B75+C75</f>
+        <f t="shared" si="11"/>
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
@@ -6284,19 +6302,19 @@
         <v>28200</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5.5999999999999995E-4</v>
       </c>
       <c r="F76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.4502491083193609</v>
       </c>
       <c r="M76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>28200</v>
       </c>
       <c r="N76" s="1">
-        <f>B76+C76</f>
+        <f t="shared" si="11"/>
         <v>5.5999999999999995E-4</v>
       </c>
     </row>
@@ -6308,19 +6326,19 @@
         <v>8630</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.4E-3</v>
       </c>
       <c r="F77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.9360107957152097</v>
       </c>
       <c r="M77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>8630</v>
       </c>
       <c r="N77" s="1">
-        <f>B77+C77</f>
+        <f t="shared" si="11"/>
         <v>1.4E-3</v>
       </c>
     </row>
@@ -6332,19 +6350,19 @@
         <v>26700</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="F78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.426511261364575</v>
       </c>
       <c r="M78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>26700</v>
       </c>
       <c r="N78" s="1">
-        <f>B78+C78</f>
+        <f t="shared" si="11"/>
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
@@ -6356,19 +6374,19 @@
         <v>388</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.2000000000000002E-3</v>
       </c>
       <c r="F79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.5888317255942073</v>
       </c>
       <c r="M79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>388</v>
       </c>
       <c r="N79" s="1">
-        <f>B79+C79</f>
+        <f t="shared" si="11"/>
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
@@ -6380,19 +6398,19 @@
         <v>42200</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.5999999999999999E-3</v>
       </c>
       <c r="F80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.6253124509616734</v>
       </c>
       <c r="M80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>42200</v>
       </c>
       <c r="N80" s="1">
-        <f>B80+C80</f>
+        <f t="shared" si="11"/>
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
@@ -6404,19 +6422,19 @@
         <v>343</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.8000000000000005E-4</v>
       </c>
       <c r="F81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.5352941200427703</v>
       </c>
       <c r="M81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>343</v>
       </c>
       <c r="N81" s="1">
-        <f>B81+C81</f>
+        <f t="shared" si="11"/>
         <v>6.8000000000000005E-4</v>
       </c>
     </row>
@@ -6428,19 +6446,19 @@
         <v>80900</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.4E-3</v>
       </c>
       <c r="F82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.9079485216122727</v>
       </c>
       <c r="M82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>80900</v>
       </c>
       <c r="N82" s="1">
-        <f>B82+C82</f>
+        <f t="shared" si="11"/>
         <v>1.4E-3</v>
       </c>
     </row>
@@ -6452,19 +6470,19 @@
         <v>39000</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.4000000000000002E-4</v>
       </c>
       <c r="F83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.5910646070264995</v>
       </c>
       <c r="M83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>39000</v>
       </c>
       <c r="N83" s="1">
-        <f>B83+C83</f>
+        <f t="shared" si="11"/>
         <v>3.4000000000000002E-4</v>
       </c>
     </row>
@@ -6476,19 +6494,19 @@
         <v>12300</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="F84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.0899051114393981</v>
       </c>
       <c r="M84">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>12300</v>
       </c>
       <c r="N84" s="1">
-        <f>B84+C84</f>
+        <f t="shared" si="11"/>
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
@@ -6500,19 +6518,19 @@
         <v>19100</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>4.7000000000000002E-3</v>
       </c>
       <c r="F85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.2810333672477272</v>
       </c>
       <c r="M85">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>19100</v>
       </c>
       <c r="N85" s="1">
-        <f>B85+C85</f>
+        <f t="shared" si="11"/>
         <v>4.7000000000000002E-3</v>
       </c>
     </row>
@@ -6524,19 +6542,19 @@
         <v>1240</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>2.3000000000000001E-4</v>
       </c>
       <c r="F86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.0934216851622351</v>
       </c>
       <c r="M86">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1240</v>
       </c>
       <c r="N86" s="1">
-        <f>B86+C86</f>
+        <f t="shared" si="11"/>
         <v>2.3000000000000001E-4</v>
       </c>
     </row>
@@ -6548,19 +6566,19 @@
         <v>1410</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="F87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.1492191126553797</v>
       </c>
       <c r="M87">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1410</v>
       </c>
       <c r="N87" s="1">
-        <f>B87+C87</f>
+        <f t="shared" si="11"/>
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
@@ -6572,19 +6590,19 @@
         <v>43500</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>3.5E-4</v>
       </c>
       <c r="F88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.638489256954637</v>
       </c>
       <c r="M88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>43500</v>
       </c>
       <c r="N88" s="1">
-        <f>B88+C88</f>
+        <f t="shared" si="11"/>
         <v>3.5E-4</v>
       </c>
     </row>
@@ -6596,19 +6614,19 @@
         <v>43500</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>5.6999999999999998E-4</v>
       </c>
       <c r="F89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.638489256954637</v>
       </c>
       <c r="M89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>43500</v>
       </c>
       <c r="N89" s="1">
-        <f>B89+C89</f>
+        <f t="shared" si="11"/>
         <v>5.6999999999999998E-4</v>
       </c>
     </row>
@@ -6620,26 +6638,26 @@
         <v>75700</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="12"/>
         <v>7.5000000000000002E-4</v>
       </c>
       <c r="F90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.8790958795000732</v>
       </c>
       <c r="M90">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>75700</v>
       </c>
       <c r="N90" s="1">
-        <f>B90+C90</f>
+        <f t="shared" si="11"/>
         <v>7.5000000000000002E-4</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="92" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>